<commit_message>
提交一批年前完成的题目: 724, 766, 989, 1052,1128
</commit_message>
<xml_diff>
--- a/总结.xlsx
+++ b/总结.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\root\LeetCode-Cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F07C6-56A6-46D8-91FD-B35C86FBD2B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBC94FD-4DE0-41B7-8D86-98EE7E5C82E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="304">
   <si>
     <t>2刷</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1297,15 +1297,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>图，最小生成树</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>三个数的最大乘积</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>排名：41178</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排名：40931</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到最小生成树里的关键边和伪关键边</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图，最小生成树，并查集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寻找数组的中心索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>托普利茨矩阵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数组形式的整数加法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爱生气的书店老板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等价多米诺骨牌的数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1790,11 +1818,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N201"/>
+  <dimension ref="A1:N207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N202" sqref="N202"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1803,7 +1831,7 @@
     <col min="2" max="2" width="6.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.25" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.75" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.75" style="1" bestFit="1" customWidth="1"/>
@@ -5043,7 +5071,7 @@
         <v>94</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="N200" s="18" t="s">
         <v>293</v>
@@ -5057,7 +5085,7 @@
         <v>628</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>14</v>
@@ -5066,7 +5094,111 @@
         <v>15</v>
       </c>
       <c r="N201" s="17" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A202" s="13">
+        <v>43851</v>
+      </c>
+      <c r="B202" s="16">
+        <v>1489</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="N202" s="17" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A203" s="13">
+        <v>44218</v>
+      </c>
+      <c r="B203" s="16">
+        <v>989</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="N203" s="17"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A204" s="13">
+        <v>44222</v>
+      </c>
+      <c r="B204" s="16">
+        <v>1128</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N204" s="17"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A205" s="13">
+        <v>44224</v>
+      </c>
+      <c r="B205" s="16">
+        <v>724</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A206" s="13">
+        <v>44249</v>
+      </c>
+      <c r="B206" s="16">
+        <v>766</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A207" s="13">
+        <v>44250</v>
+      </c>
+      <c r="B207" s="16">
+        <v>1052</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -5302,8 +5434,14 @@
     <hyperlink ref="B199" r:id="rId198" display="721" xr:uid="{A901D0AF-446F-4FE0-89AF-48124F99BFF6}"/>
     <hyperlink ref="B200" r:id="rId199" display="1584" xr:uid="{DEF8B74B-FF70-4395-BF3A-BFDE4C46B924}"/>
     <hyperlink ref="B201" r:id="rId200" display="628" xr:uid="{D2E1A981-A6BB-41FD-86C4-836B5635AFD2}"/>
+    <hyperlink ref="B202" r:id="rId201" display="1489" xr:uid="{9F97434A-F3FA-4D3C-A56F-9E9944BE8547}"/>
+    <hyperlink ref="B205" r:id="rId202" display="724" xr:uid="{9FA5AB0F-C6FD-4210-8306-5A2B250A55ED}"/>
+    <hyperlink ref="B206" r:id="rId203" display="766" xr:uid="{E02993E2-6010-41BD-A792-11014C1F9C19}"/>
+    <hyperlink ref="B203" r:id="rId204" display="989" xr:uid="{553489B8-8989-41FB-9EAC-0E9A89A852C9}"/>
+    <hyperlink ref="B207" r:id="rId205" display="1052" xr:uid="{46AEBFCC-C6FA-4982-BEF7-72673EA49D64}"/>
+    <hyperlink ref="B204" r:id="rId206" display="1128" xr:uid="{55731347-36D6-496F-A01C-5EF02C7469C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId201"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId207"/>
 </worksheet>
 </file>
</xml_diff>